<commit_message>
calculate radar 24ghz design patch, model and simulation
</commit_message>
<xml_diff>
--- a/Analysis/Sensor/Radar_MotionDetect_Parts.xlsx
+++ b/Analysis/Sensor/Radar_MotionDetect_Parts.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="121">
   <si>
     <t>Name</t>
   </si>
@@ -371,9 +371,6 @@
     <t>ATA855</t>
   </si>
   <si>
-    <t>System : PIC32MM + MRF89XA + K-LC1a</t>
-  </si>
-  <si>
     <t>MRF89XA</t>
   </si>
   <si>
@@ -381,6 +378,18 @@
   </si>
   <si>
     <t>System : XMC4300 + ATA855 + BGT24</t>
+  </si>
+  <si>
+    <t>PIC32MX470</t>
+  </si>
+  <si>
+    <t>512K</t>
+  </si>
+  <si>
+    <t>128K</t>
+  </si>
+  <si>
+    <t>System : PIC32MX470 + MRF89XA + K-LC1a</t>
   </si>
 </sst>
 </file>
@@ -6069,7 +6078,7 @@
   <dimension ref="A1:V79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6445,7 +6454,7 @@
         <v>2</v>
       </c>
       <c r="P16">
-        <f t="shared" ref="P16:P21" si="3">(1/B16)/(K16*(POWER(10,-9)))*3600</f>
+        <f t="shared" ref="P16:P22" si="3">(1/B16)/(K16*(POWER(10,-9)))*3600</f>
         <v>7199999999.999999</v>
       </c>
       <c r="Q16">
@@ -6512,27 +6521,27 @@
         <v>13235294117.647058</v>
       </c>
       <c r="Q17">
-        <f t="shared" ref="Q17:Q21" si="4">P17/86400</f>
+        <f t="shared" ref="Q17:Q22" si="4">P17/86400</f>
         <v>153186.27450980392</v>
       </c>
       <c r="R17">
-        <f t="shared" ref="R17:R21" si="5">Q17/365</f>
+        <f t="shared" ref="R17:R22" si="5">Q17/365</f>
         <v>419.68842331453129</v>
       </c>
       <c r="S17">
-        <f t="shared" ref="S17:S21" si="6">(1/B17)/(C17*(POWER(10,-3)))*3600</f>
+        <f t="shared" ref="S17:S22" si="6">(1/B17)/(C17*(POWER(10,-3)))*3600</f>
         <v>163636.36363636365</v>
       </c>
       <c r="T17">
-        <f t="shared" ref="T17:T21" si="7">S17/(POWER(10,-3)*D17)</f>
+        <f t="shared" ref="T17:T22" si="7">S17/(POWER(10,-3)*D17)</f>
         <v>14876033.057851242</v>
       </c>
       <c r="U17">
-        <f t="shared" ref="U17:U21" si="8">T17*$B$9</f>
+        <f t="shared" ref="U17:U22" si="8">T17*$B$9</f>
         <v>7438016.528925621</v>
       </c>
       <c r="V17">
-        <f t="shared" ref="V17:V21" si="9">U17/86400</f>
+        <f t="shared" ref="V17:V22" si="9">U17/86400</f>
         <v>86.088154269972463</v>
       </c>
     </row>
@@ -6779,6 +6788,63 @@
         <v>23.148148148148145</v>
       </c>
     </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>60</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" t="s">
+        <v>118</v>
+      </c>
+      <c r="H22" t="s">
+        <v>119</v>
+      </c>
+      <c r="K22">
+        <v>50000</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="3"/>
+        <v>72000000</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="4"/>
+        <v>833.33333333333337</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="5"/>
+        <v>2.2831050228310503</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="6"/>
+        <v>60000.000000000007</v>
+      </c>
+      <c r="T22">
+        <f>S22/(POWER(10,-3)*D22)</f>
+        <v>6000000.0000000009</v>
+      </c>
+      <c r="U22">
+        <f>T22*$B$9</f>
+        <v>3000000.0000000005</v>
+      </c>
+      <c r="V22">
+        <f>U22/86400</f>
+        <v>34.722222222222229</v>
+      </c>
+    </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
@@ -7143,7 +7209,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B59" t="s">
         <v>110</v>
@@ -7159,7 +7225,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B61">
         <v>180.37518037518035</v>
@@ -7167,7 +7233,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B62">
         <v>17.536475869809202</v>
@@ -7175,7 +7241,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B76" t="s">
         <v>110</v>

</xml_diff>